<commit_message>
anika tutorial and time tbale update
</commit_message>
<xml_diff>
--- a/kcl-2016/TimeTable.7BBG2014.M7.Bioinformatics.Genomic.Medicine.Feb.2016.xlsx
+++ b/kcl-2016/TimeTable.7BBG2014.M7.Bioinformatics.Genomic.Medicine.Feb.2016.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="23580" yWindow="960" windowWidth="23940" windowHeight="25900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Module.Schedule" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="78">
   <si>
     <t>Bioinformatics, Interpretation and Data Quality in Genome Analysis</t>
   </si>
@@ -245,9 +245,6 @@
   </si>
   <si>
     <t>Extraction of clinical information from electronic health records</t>
-  </si>
-  <si>
-    <t>Phenome Central and Phenotips Papers : group presentations &amp; Discussion</t>
   </si>
   <si>
     <t>Location for Lectures and Tutorials</t>
@@ -430,9 +427,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -485,13 +483,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -824,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1524,7 +1523,7 @@
         <v>47</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="E53" s="13" t="s">
         <v>56</v>
@@ -1720,17 +1719,17 @@
   <sheetData>
     <row r="1" spans="1:2" ht="24">
       <c r="A1" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18">
       <c r="A2" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18">
       <c r="A3" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16">

</xml_diff>

<commit_message>
updates Time tabke and hand book
</commit_message>
<xml_diff>
--- a/kcl-2016/TimeTable.7BBG2014.M7.Bioinformatics.Genomic.Medicine.Feb.2016.xlsx
+++ b/kcl-2016/TimeTable.7BBG2014.M7.Bioinformatics.Genomic.Medicine.Feb.2016.xlsx
@@ -829,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>